<commit_message>
1st User story element complete
</commit_message>
<xml_diff>
--- a/Domain_Model.xlsx
+++ b/Domain_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vytisvadoklis/Desktop/takeaway-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF4D61D-0A16-A042-B8C7-5DBA2E4D7BC4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7355B4E-4632-7448-A05E-3EC8522583F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t xml:space="preserve">Messages </t>
   </si>
   <si>
-    <t>TakeAway</t>
+    <t>Takeaway</t>
   </si>
   <si>
-    <t>see_list_of_dishes; select_available_dishes; check_total; text_msg;</t>
+    <t xml:space="preserve">print_menu; </t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,7 +443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>